<commit_message>
done useContext + useReducer
</commit_message>
<xml_diff>
--- a/ReactJS.xlsx
+++ b/ReactJS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOANDO\Desktop\ReacJs-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E0948E-C821-47DB-9CB3-467AC6DEEE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430989EC-324E-421F-9B38-7A2369783B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14745" yWindow="585" windowWidth="14055" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16875" yWindow="600" windowWidth="14055" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chuẩn bị" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="157">
   <si>
     <t>I) Cách tạo 1 project với reactjs</t>
   </si>
@@ -470,6 +470,45 @@
   </si>
   <si>
     <t>- Hoạt động theo các bước sau:</t>
+  </si>
+  <si>
+    <t>- Tạo một ngữ cảnh (Context) để ôm component cha và từ đó nó có truyền dữ liệu tới bất kỳ component con nào, để làm được điều đó nó sử dụng Provider</t>
+  </si>
+  <si>
+    <t>- Tại Component cha</t>
+  </si>
+  <si>
+    <t>- Component con:</t>
+  </si>
+  <si>
+    <t>- Sử dụng children để đánh dấu nội dung con sẽ được truyền vào</t>
+  </si>
+  <si>
+    <t>9. Context + useReducer =&gt; global state</t>
+  </si>
+  <si>
+    <t>- Vì state để ở global nên có thể sẽ có rất nhiều state vậy nên ta sử dụng useReducer thay vì sử dung useState</t>
+  </si>
+  <si>
+    <t>10. Custom 1 hook</t>
+  </si>
+  <si>
+    <t>11. So sánh Redux với React-context</t>
+  </si>
+  <si>
+    <t>- Debugging capabilities</t>
+  </si>
+  <si>
+    <t>- Middleware</t>
+  </si>
+  <si>
+    <t>- Addons and extensibility</t>
+  </si>
+  <si>
+    <t>- cross-platform and cross-framework usage</t>
+  </si>
+  <si>
+    <t>- Depending on your app's setup, much better performance than working with jusst Context</t>
   </si>
 </sst>
 </file>
@@ -560,6 +599,810 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>53242</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>124480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA0C01B6-7D98-1733-923E-29C7A5F6180E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1821656" y="32194500"/>
+          <a:ext cx="6125430" cy="4696480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>404813</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>130969</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>178593</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D8E20DD-4F7A-3FA9-E0D9-0177C9FD8865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2226469" y="33087469"/>
+          <a:ext cx="3417093" cy="309562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>283369</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>226218</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6028B267-67D9-4718-826B-4A837430A8F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2712244" y="34704338"/>
+          <a:ext cx="2978943" cy="309562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>59530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Speech Bubble: Rectangle with Corners Rounded 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{883D3E2C-92B7-AF78-6257-3ECF725157DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5679281" y="33778030"/>
+          <a:ext cx="1821656" cy="750094"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -50898"/>
+            <a:gd name="adj2" fmla="val 79960"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>value là</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> dữ liệu cần truyền tới các component con</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>588843</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>9952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{916E349A-A518-16E3-C769-3FA62004D1C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1821656" y="37528500"/>
+          <a:ext cx="4839375" cy="3057952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C67710F5-CE65-4009-A7B9-AFBD61123BFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2571750" y="38361937"/>
+          <a:ext cx="2978943" cy="309562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571498</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Speech Bubble: Rectangle with Corners Rounded 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{140CBD22-15AE-485F-9678-7400E53289C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5429248" y="37409437"/>
+          <a:ext cx="2750345" cy="750094"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -50898"/>
+            <a:gd name="adj2" fmla="val 79960"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>useContext</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> của create context của component cha và từ đó lấy đc dữ liệu của component cha {theme}</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>167559</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>114741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB2E6E9-CA31-7720-117A-8C9DA1A0D67D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1214438" y="41910000"/>
+          <a:ext cx="6239746" cy="3162741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>250031</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>178593</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>192881</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>107155</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{437286F9-DF40-4D3F-9A08-A0A58900DC07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1464469" y="42088593"/>
+          <a:ext cx="2978943" cy="309562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>259554</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>21431</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Speech Bubble: Rectangle with Corners Rounded 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C39AD08-509E-4449-8279-C362067F8AD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4510085" y="41181337"/>
+          <a:ext cx="2750345" cy="750094"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -50898"/>
+            <a:gd name="adj2" fmla="val 79960"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>để</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> sử dụng context luôn phải import 2 thằng này =&gt; custom hook để import một thằng là đc</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>181766</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD191DB9-13ED-9E04-AF6A-72AEECF0A4C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="3619500"/>
+          <a:ext cx="5668166" cy="3943900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>226218</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4879176-8318-4F99-BA87-13FBA9FA8D7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1514475" y="4324350"/>
+          <a:ext cx="2978943" cy="309562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB602658-3A0A-4255-97AC-C197C410CFD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2371725" y="6019799"/>
+          <a:ext cx="1381125" cy="190501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,10 +1748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:G164"/>
+  <dimension ref="B2:G245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K155" sqref="K155"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,9 +2498,70 @@
         <v>142</v>
       </c>
     </row>
+    <row r="166" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C166" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="168" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C168" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C196" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C217" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B239" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C241" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C242" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C243" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C244" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C245" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1714,10 +2618,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F76A81E-C35A-40D0-887C-046B85BCBB6A}">
-  <dimension ref="B2:D16"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:I16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +2697,13 @@
         <v>133</v>
       </c>
     </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tìm hiểu về router
</commit_message>
<xml_diff>
--- a/ReactJS.xlsx
+++ b/ReactJS.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOANDO\Desktop\ReacJs-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4317968C-CC54-4EBB-8AFB-CB327A2FF8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9C176F-CB85-47AE-BB55-08B5995EAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15975" yWindow="2040" windowWidth="14055" windowHeight="11295" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chuẩn bị" sheetId="1" r:id="rId1"/>
     <sheet name="HOOK" sheetId="2" r:id="rId2"/>
     <sheet name="Memo" sheetId="4" r:id="rId3"/>
     <sheet name="Css" sheetId="5" r:id="rId4"/>
-    <sheet name="Chú ý" sheetId="3" r:id="rId5"/>
+    <sheet name="Router" sheetId="6" r:id="rId5"/>
+    <sheet name="JWT" sheetId="7" r:id="rId6"/>
+    <sheet name="Chú ý" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="232">
   <si>
     <t>I) Cách tạo 1 project với reactjs</t>
   </si>
@@ -635,12 +637,185 @@
   <si>
     <t>- Prop className nhận kiểu dữ liệu là chuỗi</t>
   </si>
+  <si>
+    <t>4, SASS</t>
+  </si>
+  <si>
+    <t>- install Sass: npm add sass</t>
+  </si>
+  <si>
+    <t>- Cho bạn di chuyển qua lại giữa các trang trong website</t>
+  </si>
+  <si>
+    <t>2. reactjs router</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- install: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>npm install react-router-dom@6</t>
+    </r>
+  </si>
+  <si>
+    <t>Cách sử dụng:</t>
+  </si>
+  <si>
+    <t>- B1: Import BrowserRouter</t>
+  </si>
+  <si>
+    <t>- B2: Ôm component App trong BrowserRouter</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chú ý</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: một website chỉ có một bộ định tuyến thôi (tức là một BrowserRouter)</t>
+    </r>
+  </si>
+  <si>
+    <t>- B3: trong App Component:</t>
+  </si>
+  <si>
+    <t>- Tạo ra cơ chế định tuyến nội bộ trong reactjs</t>
+  </si>
+  <si>
+    <t>- exact: match chính xác đường dẫn</t>
+  </si>
+  <si>
+    <t>- path='*' những đường dẫn còn lại khác các đường dẫn đã cấu hình</t>
+  </si>
+  <si>
+    <t>3. Nested Route</t>
+  </si>
+  <si>
+    <t>- Tạo các submenu lồng nhau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ B1: </t>
+  </si>
+  <si>
+    <t>+ B2: Tạo Component AdminPage và cấu hình các route con bên trong là xong</t>
+  </si>
+  <si>
+    <t>4. Đọc Params, History, Location</t>
+  </si>
+  <si>
+    <t>- Location:</t>
+  </si>
+  <si>
+    <t>+ import hook trong react-router-dom là useLocation() hoặc useRouteMatch() để đọc pathname</t>
+  </si>
+  <si>
+    <t>- Đọc Params:</t>
+  </si>
+  <si>
+    <t>+ Sử dụng useLocation để đọc params</t>
+  </si>
+  <si>
+    <t>+ B1: let location = useLocation();</t>
+  </si>
+  <si>
+    <t>+ B2:let query = new URLSearchParams(location.search)</t>
+  </si>
+  <si>
+    <t>+ B3: Lấy ra {quert.get('param_name')}</t>
+  </si>
+  <si>
+    <t>TH1: đối với cách truyền param ?name=doan&amp;id=1</t>
+  </si>
+  <si>
+    <t>TH2: đối với cách truyền param category/:id</t>
+  </si>
+  <si>
+    <t>+ B1: let {id} = useParams()</t>
+  </si>
+  <si>
+    <t>- History:</t>
+  </si>
+  <si>
+    <t>+ Để back lại trang trước đó ta sử dụng hook useHistory()</t>
+  </si>
+  <si>
+    <t>+ B1: const history = useHistory()</t>
+  </si>
+  <si>
+    <t>+ B2: onClick={() =&gt; history.goBack()}</t>
+  </si>
+  <si>
+    <t>Để chuyển về một trang khác</t>
+  </si>
+  <si>
+    <t>+ B2: onClick={() =&gt; history.push('home')}</t>
+  </si>
+  <si>
+    <t>5. Xử lý giao diện Active Link Style</t>
+  </si>
+  <si>
+    <t>- Để check link người dùng chọn có khớp vs link hiện tại ko ta sử dụng</t>
+  </si>
+  <si>
+    <t>+ B1: const match = useRouterMatch({</t>
+  </si>
+  <si>
+    <t>path: item.path</t>
+  </si>
+  <si>
+    <t>})</t>
+  </si>
+  <si>
+    <t>=&gt; đối tượng match trả về null nếu ko tìm thấy</t>
+  </si>
+  <si>
+    <t>+ B2: className={match ? 'active' : 'inactive'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Gồm 3 phần: </t>
+  </si>
+  <si>
+    <t>+ Header: bao gồm thuật toán mã hóa và type là JWT</t>
+  </si>
+  <si>
+    <t>+ Payload: data cần truyền đi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Signature: mã hóa base64 header và payload từ đó mã hóa </t>
+  </si>
+  <si>
+    <t>- Cơ chế refresh token để bảo mật</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,13 +870,27 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -716,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -731,12 +920,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1734,6 +1925,664 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>515185</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>143641</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE10D9BE-A5A7-52E9-7661-C28D7C31E97C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2457450" y="2847975"/>
+          <a:ext cx="5982535" cy="5487166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>467471</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>48456</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F77FBCD8-ADF1-4665-0ABD-0FEF65E46E4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="9334500"/>
+          <a:ext cx="5344271" cy="5953956"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCF0E239-00B4-8066-4628-7B935702E550}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2505075" y="9334500"/>
+          <a:ext cx="4591050" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4E2990-3A45-4EB3-BB30-3EF96626E05A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3352801" y="13306426"/>
+          <a:ext cx="742950" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A17EBC1D-9552-4584-ADDF-167C2BF3DFEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3724275" y="13515975"/>
+          <a:ext cx="3752849" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Speech Bubble: Rectangle with Corners Rounded 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D831AD-FDEE-B3F6-2A09-8EBE83110E4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7210425" y="9334501"/>
+          <a:ext cx="1562100" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -56237"/>
+            <a:gd name="adj2" fmla="val -37500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Import</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> các thành phần cần thiết</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Speech Bubble: Rectangle with Corners Rounded 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F965B8DF-6872-4104-ACD9-922739891D02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6229349" y="11344276"/>
+          <a:ext cx="3952875" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -56237"/>
+            <a:gd name="adj2" fmla="val -37500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Để</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> link chuyển page ta sử dụng Link và to đến path chúng ta muốn</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>=&gt; Khi render nó sẽ render Link -&gt; thẻ a</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Speech Bubble: Rectangle with Corners Rounded 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EECA283A-C453-4401-90BA-0DEDCBC91DFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7715250" y="13535026"/>
+          <a:ext cx="3181350" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -56237"/>
+            <a:gd name="adj2" fmla="val -37500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Định</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> nghĩa:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  + path: đường đẫn url</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  + element: react element tương ứng</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>153187</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>162213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{494A6C72-E9B7-5638-D1C6-7055BAC8BBDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="17145000"/>
+          <a:ext cx="5639587" cy="2067213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CCD6EF9-1CC3-7B39-E445-5AF78C00F4C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="18126075"/>
+          <a:ext cx="3705225" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3166,10 +4015,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0247A594-4926-4C5F-9AD3-F25456BFA155}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:H27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3255,13 +4104,23 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>187</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3273,11 +4132,291 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFC9925-76D0-4E3D-A748-E27ED063F45B}">
+  <dimension ref="B2:I135"/>
+  <sheetViews>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="G136" sqref="G136"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C107" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D108" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C110" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D112" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D117" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E117" s="11"/>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
+      <c r="H117" s="11"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D118" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C120" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D121" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+      <c r="G121" s="11"/>
+      <c r="H121" s="11"/>
+      <c r="I121" s="11"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D123" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D125" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E125" s="11"/>
+      <c r="F125" s="11"/>
+      <c r="G125" s="11"/>
+      <c r="H125" s="11"/>
+      <c r="I125" s="11"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D126" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C130" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D131" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D134" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D135" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1457756D-6193-4F21-9DC9-23B984F4E6B2}">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F76A81E-C35A-40D0-887C-046B85BCBB6A}">
   <dimension ref="B2:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,30 +4498,30 @@
       </c>
     </row>
     <row r="42" spans="2:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
     </row>
     <row r="44" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">

</xml_diff>

<commit_message>
ap dung thu vien PropTypes
</commit_message>
<xml_diff>
--- a/ReactJS.xlsx
+++ b/ReactJS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOANDO\Desktop\ReacJs-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A73BB13-077E-4383-87DE-D5F2C67568B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36683672-0482-46DD-AE55-19A8D52E3CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14655" yWindow="1695" windowWidth="14055" windowHeight="11295" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17040" yWindow="1500" windowWidth="14055" windowHeight="11295" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chuẩn bị" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="348">
   <si>
     <t>I) Cách tạo 1 project với reactjs</t>
   </si>
@@ -2462,6 +2462,27 @@
   </si>
   <si>
     <t>- appendTo={() =&gt; document.body}</t>
+  </si>
+  <si>
+    <t>- Các môi trường phát triển</t>
+  </si>
+  <si>
+    <t>+ Local/development</t>
+  </si>
+  <si>
+    <t>+ Test/Staging</t>
+  </si>
+  <si>
+    <t>+ Production</t>
+  </si>
+  <si>
+    <t>+ UAT</t>
+  </si>
+  <si>
+    <t>8. Tìm hiểu thư viện PropTypes</t>
+  </si>
+  <si>
+    <t>- import PropTypes from 'prop-types'</t>
   </si>
 </sst>
 </file>
@@ -6786,10 +6807,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC586F05-E1D9-4BD2-A973-9FB851DCD088}">
-  <dimension ref="B2:L232"/>
+  <dimension ref="B2:L235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="I234" sqref="I234"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="E239" sqref="E239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7550,13 +7571,23 @@
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B231" t="s">
+      <c r="B231" s="1" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C232" s="2" t="s">
         <v>318</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B234" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C235" s="2" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -7613,10 +7644,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F76A81E-C35A-40D0-887C-046B85BCBB6A}">
-  <dimension ref="B2:J53"/>
+  <dimension ref="B2:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M69" sqref="M69"/>
+    <sheetView topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7746,6 +7777,31 @@
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xây dựng phần sidebar
</commit_message>
<xml_diff>
--- a/ReactJS.xlsx
+++ b/ReactJS.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="354">
   <si>
     <t>I) Cách tạo 1 project với reactjs</t>
   </si>
@@ -2485,13 +2485,326 @@
   </si>
   <si>
     <t>6. Để xử lý thằng link nào đc active ta sử dụng NavLink</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Cơ chế hoạt động: nó sẽ so sánh thằng </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> trên url với thằng prop </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>và nó sẽ tự  thêm class active nếu nó trùng nhau</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NavLink</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>className</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'menu-item'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>active:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>nav</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>isActive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>})</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>+ thằng nav và nav.isActive ở đâu ra thì nó là của thằng NavLink</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>- Để css active trong module.scss thì ta phải chuyển nó về dạng cx thì mới viết scss đc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2653,6 +2966,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2704,7 +3031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2747,6 +3074,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6574,10 +6904,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I137"/>
+  <dimension ref="B2:L144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="K144" sqref="K144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6770,39 +7100,73 @@
         <v>220</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C130" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D131" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E132" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D134" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D135" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C138" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C139" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C140" s="23" t="s">
+        <v>350</v>
+      </c>
+      <c r="D140" s="15"/>
+      <c r="E140" s="15"/>
+      <c r="F140" s="15"/>
+      <c r="G140" s="15"/>
+      <c r="H140" s="15"/>
+      <c r="I140" s="15"/>
+      <c r="J140" s="15"/>
+      <c r="K140" s="15"/>
+      <c r="L140" s="15"/>
+    </row>
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D141" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F144" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>